<commit_message>
Added test cases, fixed methods to allow filepath arg
</commit_message>
<xml_diff>
--- a/testFiles/empty.xlsx
+++ b/testFiles/empty.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -396,162 +396,9 @@
         <v>A</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3" t="str">
-        <v>A</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="B4" t="str">
-        <v>A</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5">
-        <v>3</v>
-      </c>
-      <c r="B5" t="str">
-        <v>A</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6">
-        <v>4</v>
-      </c>
-      <c r="B6" t="str">
-        <v>A</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7">
-        <v>5</v>
-      </c>
-      <c r="B7" t="str">
-        <v>A</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8">
-        <v>6</v>
-      </c>
-      <c r="B8" t="str">
-        <v>A</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9">
-        <v>7</v>
-      </c>
-      <c r="B9" t="str">
-        <v>A</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10">
-        <v>8</v>
-      </c>
-      <c r="B10" t="str">
-        <v>A</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11">
-        <v>9</v>
-      </c>
-      <c r="B11" t="str">
-        <v>A</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12">
-        <v>10</v>
-      </c>
-      <c r="B12" t="str">
-        <v>A</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13">
-        <v>11</v>
-      </c>
-      <c r="B13" t="str">
-        <v>A</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14">
-        <v>12</v>
-      </c>
-      <c r="B14" t="str">
-        <v>A</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15">
-        <v>13</v>
-      </c>
-      <c r="B15" t="str">
-        <v>A</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16">
-        <v>14</v>
-      </c>
-      <c r="B16" t="str">
-        <v>A</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17">
-        <v>15</v>
-      </c>
-      <c r="B17" t="str">
-        <v>A</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18">
-        <v>16</v>
-      </c>
-      <c r="B18" t="str">
-        <v>A</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19">
-        <v>17</v>
-      </c>
-      <c r="B19" t="str">
-        <v>A</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20">
-        <v>18</v>
-      </c>
-      <c r="B20" t="str">
-        <v>A</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21">
-        <v>19</v>
-      </c>
-      <c r="B21" t="str">
-        <v>A</v>
-      </c>
-    </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:B21"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:B2"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>